<commit_message>
all kinds of STUFF
but notable the Longevity business for working on at home
(for Alex's presentation)
</commit_message>
<xml_diff>
--- a/longevity/Yerkes aggregation/Copy of CHIMP RemovalsDeaths1.xlsx
+++ b/longevity/Yerkes aggregation/Copy of CHIMP RemovalsDeaths1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="325">
   <si>
     <t>Subject</t>
   </si>
@@ -996,6 +996,9 @@
   </si>
   <si>
     <t>LTF</t>
+  </si>
+  <si>
+    <t>these two columns are WRONG</t>
   </si>
 </sst>
 </file>
@@ -1384,7 +1387,7 @@
   <dimension ref="A1:K176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1423,6 +1426,9 @@
         <v>303</v>
       </c>
       <c r="H1" s="2"/>
+      <c r="J1" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">

</xml_diff>